<commit_message>
update english overview template
</commit_message>
<xml_diff>
--- a/src/spz/templates/export/english_overview.xlsx
+++ b/src/spz/templates/export/english_overview.xlsx
@@ -10,9 +10,6 @@
   <sheets>
     <sheet name="Kursliste" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Kursliste!$A$1:$H$2</definedName>
-  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -23,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t xml:space="preserve">Vorname</t>
   </si>
@@ -40,6 +37,9 @@
     <t xml:space="preserve">Level</t>
   </si>
   <si>
+    <t xml:space="preserve">Ilias Test (%)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Semester</t>
   </si>
   <si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t xml:space="preserve">applicant.get_test_ger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">applicant.best_rating()</t>
   </si>
   <si>
     <t xml:space="preserve">semester</t>
@@ -80,7 +83,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -107,6 +110,14 @@
       <b val="true"/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -191,7 +202,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -205,6 +216,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -311,21 +330,19 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="DATA" displayName="DATA" ref="A1:G2" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:G2"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="DATA" displayName="DATA" ref="A1:I2" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:I2"/>
+  <tableColumns count="9">
     <tableColumn id="1" name="Vorname"/>
     <tableColumn id="2" name="Nachname"/>
     <tableColumn id="3" name="Matrikelnummer"/>
     <tableColumn id="4" name="Kurs"/>
     <tableColumn id="5" name="Level"/>
-    <tableColumn id="6" name="Semester"/>
-    <tableColumn id="7" name="Note (%)"/>
+    <tableColumn id="6" name="Ilias Test (%)"/>
+    <tableColumn id="7" name="Semester"/>
+    <tableColumn id="8" name="Note (%)"/>
+    <tableColumn id="9" name="Gesamtnote"/>
   </tableColumns>
 </table>
 </file>
@@ -335,25 +352,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
+      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="21.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="19.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="22.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="27.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.72"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -372,41 +389,58 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="0" t="s">
         <v>14</v>
       </c>
+      <c r="G2" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="H2" s="0" t="s">
-        <v>15</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G9" s="4"/>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C11" s="5"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H2"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -414,9 +448,8 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <drawing r:id="rId1"/>
   <tableParts>
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update overview excel templates
</commit_message>
<xml_diff>
--- a/src/spz/templates/export/english_overview.xlsx
+++ b/src/spz/templates/export/english_overview.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfenker\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USM\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -62,9 +62,6 @@
     <t>applicant.tag</t>
   </si>
   <si>
-    <t>course.full_name</t>
-  </si>
-  <si>
     <t>applicant.get_test_ger</t>
   </si>
   <si>
@@ -84,6 +81,9 @@
   </si>
   <si>
     <t>LP</t>
+  </si>
+  <si>
+    <t>course.name_english</t>
   </si>
 </sst>
 </file>
@@ -549,7 +549,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -588,7 +588,7 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>7</v>
@@ -608,26 +608,29 @@
         <v>11</v>
       </c>
       <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>13</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" t="s">
         <v>15</v>
       </c>
-      <c r="H2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>16</v>
       </c>
-      <c r="J2" t="s">
-        <v>17</v>
-      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D3" s="4"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G7" s="4"/>

</xml_diff>